<commit_message>
Add new folder for Post 2026 Web Tool
</commit_message>
<xml_diff>
--- a/LakePowellNewBathymetry/Lake_Powell_Area_Capacity_Table_Report_FINAL.xlsx
+++ b/LakePowellNewBathymetry/Lake_Powell_Area_Capacity_Table_Report_FINAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakePowellNewBathymetry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498A0F5A-B356-4E08-9CA6-DA05BFD1A960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932A5D05-83C9-45DF-992C-B3D3065A43D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-1800" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,7 +322,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -429,9 +429,6 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -450,6 +447,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -25525,8 +25528,8 @@
       <c r="J4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="41"/>
-      <c r="Q4" s="41"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="28">
@@ -42733,143 +42736,144 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770C52C0-5EB3-44BC-B2AD-268DDE97C314}">
-  <dimension ref="C13:E22"/>
+  <dimension ref="C13:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:E18"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.69921875" style="42" customWidth="1"/>
-    <col min="4" max="4" width="14.59765625" style="42" customWidth="1"/>
+    <col min="3" max="3" width="11.69921875" style="41" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" style="41" customWidth="1"/>
     <col min="5" max="5" width="8.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="13" spans="3:5" ht="39" x14ac:dyDescent="0.3">
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="46" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C14" s="44">
+      <c r="C14" s="43">
         <v>3370</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="42">
         <f>VLOOKUP(C14,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="46">
+      <c r="E14" s="45">
         <f>D14/$D$22</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C15" s="44">
+      <c r="C15" s="43">
         <v>3490</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="42">
         <f>VLOOKUP(C15,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>3.7427141499999999</v>
       </c>
-      <c r="E15" s="46">
+      <c r="E15" s="45">
         <f t="shared" ref="E15:E22" si="0">D15/$D$22</f>
         <v>0.16053622836851369</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C16" s="44">
+      <c r="C16" s="43">
         <v>3500</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="42">
         <f>VLOOKUP(C16,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>4.2158051219999999</v>
       </c>
-      <c r="E16" s="46">
+      <c r="E16" s="45">
         <f t="shared" si="0"/>
         <v>0.180828518208515</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" s="44">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="43">
         <v>3525</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="42">
         <f>VLOOKUP(C17,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>5.5449229090000003</v>
       </c>
-      <c r="E17" s="46">
+      <c r="E17" s="45">
         <f t="shared" si="0"/>
         <v>0.23783836401319275</v>
       </c>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" s="44">
+      <c r="F17" s="47"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="43">
         <v>3535</v>
       </c>
-      <c r="D18" s="43">
+      <c r="D18" s="42">
         <f>VLOOKUP(C18,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>6.138470743000001</v>
       </c>
-      <c r="E18" s="46">
+      <c r="E18" s="45">
         <f t="shared" si="0"/>
         <v>0.26329740972381982</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" s="44">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="43">
         <v>3550</v>
       </c>
-      <c r="D19" s="43">
+      <c r="D19" s="42">
         <f>VLOOKUP(C19,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>7.0981696620000001</v>
       </c>
-      <c r="E19" s="46">
+      <c r="E19" s="45">
         <f t="shared" si="0"/>
         <v>0.30446177297758303</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" s="44">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="43">
         <v>3570</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="42">
         <f>VLOOKUP(C20,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>8.518031302999999</v>
       </c>
-      <c r="E20" s="46">
+      <c r="E20" s="45">
         <f t="shared" si="0"/>
         <v>0.36536389467749125</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" s="44">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="43">
         <v>3600</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="42">
         <f>VLOOKUP(C21,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>10.991147309999999</v>
       </c>
-      <c r="E21" s="46">
+      <c r="E21" s="45">
         <f t="shared" si="0"/>
         <v>0.47144325317767982</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="44">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="43">
         <v>3700</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="42">
         <f>VLOOKUP(C22,BathymetryCompare!$A$4:$C$344,2)</f>
         <v>23.313828835000002</v>
       </c>
-      <c r="E22" s="46">
+      <c r="E22" s="45">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -42903,18 +42907,18 @@
       <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="40">
+      <c r="B2" s="48">
         <v>2017</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40" t="s">
+      <c r="C2" s="48"/>
+      <c r="D2" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40" t="s">
+      <c r="E2" s="48"/>
+      <c r="F2" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="40"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:7" ht="52" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">

</xml_diff>